<commit_message>
Fixed før og efterbehandling, samt screenshot funktion!!!!!!!1
</commit_message>
<xml_diff>
--- a/Uddeholm.Test/bin/debug/PVD.xlsx
+++ b/Uddeholm.Test/bin/debug/PVD.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17702"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="A1BF80AD3BB305E75EE6715F3CA894BD2E240A94" xr6:coauthVersionLast="12" xr6:coauthVersionMax="12" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9276"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171026"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,8 +31,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,19 +440,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="30" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -459,7 +460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="4">
         <v>6</v>
       </c>
@@ -467,7 +468,7 @@
         <v>11.56</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="4">
         <v>10</v>
       </c>
@@ -475,7 +476,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="4">
         <v>15</v>
       </c>
@@ -483,7 +484,7 @@
         <v>7.59</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="4">
         <v>20</v>
       </c>
@@ -491,7 +492,7 @@
         <v>7.42</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="4">
         <v>25</v>
       </c>
@@ -499,7 +500,7 @@
         <v>6.99</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="4">
         <v>30</v>
       </c>
@@ -507,7 +508,7 @@
         <v>6.56</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="4">
         <v>35</v>
       </c>
@@ -515,7 +516,7 @@
         <v>5.95</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="4">
         <v>42</v>
       </c>
@@ -523,7 +524,7 @@
         <v>5.52</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="4">
         <v>50</v>
       </c>
@@ -531,7 +532,7 @@
         <v>5.09</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="4">
         <v>55</v>
       </c>
@@ -539,7 +540,7 @@
         <v>4.66</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="4">
         <v>65</v>
       </c>
@@ -547,7 +548,7 @@
         <v>4.3099999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="4">
         <v>70</v>
       </c>
@@ -555,7 +556,7 @@
         <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="4">
         <v>80</v>
       </c>
@@ -563,7 +564,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" s="4">
         <v>90</v>
       </c>
@@ -571,7 +572,7 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="4">
         <v>100</v>
       </c>
@@ -580,7 +581,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="4">
         <v>110</v>
       </c>
@@ -588,7 +589,7 @@
         <v>3.45</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" s="4">
         <v>120</v>
       </c>
@@ -596,7 +597,7 @@
         <v>3.28</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" s="4">
         <v>140</v>
       </c>
@@ -604,7 +605,7 @@
         <v>3.19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20" s="4">
         <v>150</v>
       </c>
@@ -612,7 +613,7 @@
         <v>3.19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
       <c r="A21" s="4">
         <v>170</v>
       </c>
@@ -620,7 +621,7 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22" s="4">
         <v>180</v>
       </c>
@@ -628,7 +629,7 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
       <c r="A23" s="4">
         <v>200</v>
       </c>
@@ -636,7 +637,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="A24" s="4">
         <v>220</v>
       </c>
@@ -644,7 +645,7 @@
         <v>2.93</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25" s="4">
         <v>250</v>
       </c>
@@ -652,7 +653,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2">
       <c r="A26" s="4">
         <v>370</v>
       </c>
@@ -660,7 +661,7 @@
         <v>2.76</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="A27" s="4">
         <v>490</v>
       </c>
@@ -668,7 +669,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2">
       <c r="A28" s="4">
         <v>620</v>
       </c>
@@ -676,7 +677,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2">
       <c r="A29" s="4">
         <v>750</v>
       </c>
@@ -684,7 +685,7 @@
         <v>2.42</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2">
       <c r="A30" s="4">
         <v>870</v>
       </c>
@@ -692,7 +693,7 @@
         <v>2.33</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2">
       <c r="A31" s="4">
         <v>930</v>
       </c>
@@ -700,7 +701,7 @@
         <v>2.2400000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2">
       <c r="A32" s="4">
         <v>1000</v>
       </c>
@@ -708,7 +709,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2">
       <c r="A33" s="4">
         <v>1100</v>
       </c>
@@ -716,7 +717,7 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2">
       <c r="A34" s="4">
         <v>1200</v>
       </c>
@@ -724,7 +725,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2">
       <c r="A35" s="4">
         <v>1300</v>
       </c>
@@ -732,7 +733,7 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2">
       <c r="A36" s="4">
         <v>1400</v>
       </c>
@@ -740,7 +741,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2">
       <c r="A37" s="4">
         <v>1500</v>
       </c>
@@ -748,7 +749,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2">
       <c r="A38" s="4">
         <v>1600</v>
       </c>
@@ -756,7 +757,7 @@
         <v>1.47</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2">
       <c r="A39" s="4">
         <v>1700</v>
       </c>
@@ -764,7 +765,7 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2">
       <c r="A40" s="4">
         <v>2000</v>
       </c>
@@ -772,7 +773,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2">
       <c r="A41" s="4">
         <v>2200</v>
       </c>
@@ -780,7 +781,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2">
       <c r="A42" s="4">
         <v>2400</v>
       </c>
@@ -788,7 +789,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2">
       <c r="A43" s="4">
         <v>2800</v>
       </c>
@@ -796,7 +797,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2">
       <c r="A44" s="4">
         <v>3200</v>
       </c>
@@ -804,7 +805,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2">
       <c r="A45" s="4">
         <v>3600</v>
       </c>
@@ -812,7 +813,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2">
       <c r="A46" s="4">
         <v>4000</v>
       </c>
@@ -820,7 +821,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2">
       <c r="A47" s="4">
         <v>5500</v>
       </c>
@@ -828,7 +829,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2">
       <c r="A48" s="4">
         <v>6500</v>
       </c>
@@ -836,7 +837,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2">
       <c r="A49" s="4">
         <v>8000</v>
       </c>
@@ -844,7 +845,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2">
       <c r="A50" s="4">
         <v>12000</v>
       </c>
@@ -852,7 +853,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2">
       <c r="A51" s="4">
         <v>20000</v>
       </c>
@@ -860,7 +861,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2">
       <c r="A52" s="4">
         <v>35000</v>
       </c>
@@ -868,7 +869,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2">
       <c r="A53" s="4">
         <v>55000</v>
       </c>
@@ -876,7 +877,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2">
       <c r="A54" s="4">
         <v>75000</v>
       </c>
@@ -884,7 +885,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2">
       <c r="A55" s="4">
         <v>100000</v>
       </c>
@@ -892,7 +893,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2">
       <c r="A56" s="4">
         <v>145000</v>
       </c>
@@ -900,7 +901,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2">
       <c r="A57" s="4">
         <v>200000</v>
       </c>

</xml_diff>